<commit_message>
try to change reports.
</commit_message>
<xml_diff>
--- a/src/main/resources/RaportS61Template.xlsx
+++ b/src/main/resources/RaportS61Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1-DEV\resource-management\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1-DEV\projects\resource-management\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C735F48-BD1E-4746-8342-6E9F3D605967}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F11E0E-DAEE-438E-924B-F49A0FAE54A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{4C94B017-F92B-4544-A4F9-72BFE0E64EDE}"/>
   </bookViews>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{AE494C65-B6BD-41A2-9976-3745C6DC3EC0}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{96D44E86-8997-4DE5-8E0B-BC46D220735D}">
       <text>
         <r>
           <rPr>
@@ -69,7 +69,8 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>CHISCARI Andreea:</t>
+          <t xml:space="preserve">CHISCARI Andreea:
+</t>
         </r>
         <r>
           <rPr>
@@ -78,12 +79,11 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">
-jx:each(items="firstInterventionResources" var="resource" lastCell="I10")</t>
+          <t>jx:each(items="firstInterventionResources" var="vehicleType" lastCell="C7" direction="RIGHT")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{04B050EF-D5A4-421A-B921-B60D47571EEE}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{F74044AC-09AD-491D-97BC-2FDC38ECFED8}">
       <text>
         <r>
           <rPr>
@@ -93,6 +93,30 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">CHISCARI Andreea:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:each(items="otherResources" var="vehicleType" lastCell="E7" direction="RIGHT")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{76B60D9B-8151-4BA4-8F20-734C983E8407}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
           <t>CHISCARI Andreea:</t>
         </r>
         <r>
@@ -103,7 +127,57 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="subUnitReports" var="report" lastCell="I10")</t>
+jx:each(items="subUnitReports" var="report" lastCell="B10")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{075263F6-0E1B-4307-85B8-13D8222D6327}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CHISCARI Andreea:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="subUnitReports" var="report" lastCell="C10")
+jx:each(items="firstInterventionResources" var="vehicleType" lastCell="C10" direction="RIGHT")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{16A611A7-7D03-49D7-BB28-8C4C5D613D83}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>CHISCARI Andreea:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="subUnitReports" var="report" lastCell="E10")
+jx:each(items="otherResources" var="vehicleType" lastCell="E10" direction="RIGHT")</t>
         </r>
       </text>
     </comment>
@@ -112,10 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
-  <si>
-    <t>Echipamente</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>TOTAL Echipamente</t>
   </si>
@@ -123,12 +194,6 @@
     <t>Garda de interventie</t>
   </si>
   <si>
-    <t>Tehnica de prima interventie</t>
-  </si>
-  <si>
-    <t>Alte tipuri de tehnica</t>
-  </si>
-  <si>
     <t>TOTAL tehnica de prima interventie</t>
   </si>
   <si>
@@ -150,29 +215,29 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>${resource.longName}</t>
-  </si>
-  <si>
     <t>TEHNICA DE INTERVENȚIE OPERAȚIONALĂ ȘI NEOPERAȚIONALĂ A I.S.U. CLUJ ÎN DATA DE ${date}</t>
   </si>
   <si>
-    <t>Tehnică de intervenție</t>
-  </si>
-  <si>
-    <t>${equipment.equipmentType}</t>
-  </si>
-  <si>
     <t>${report.subUnitName}</t>
   </si>
   <si>
-    <t>${report:getCount(report.subUnitName, 'operational', ${C7})}</t>
+    <t>${vehicleType.longName}</t>
+  </si>
+  <si>
+    <t>${report:getCount(report.subUnitName, vehicleType,'operational')}</t>
+  </si>
+  <si>
+    <t>${report:getCount(report.subUnitName, vehicleType,'rezerva')}</t>
+  </si>
+  <si>
+    <t>${report:getCount(report.subUnitName, vehicleType,'neoperational')}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,8 +287,29 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,8 +327,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -294,54 +386,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -364,62 +408,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -431,65 +424,49 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="135"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="135"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="135"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,225 +786,226 @@
   <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D11" sqref="D11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="6" max="7" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
     </row>
     <row r="2" spans="1:35" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
-      <c r="AB2" s="17"/>
-      <c r="AC2" s="17"/>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17"/>
-      <c r="AH2" s="17"/>
-      <c r="AI2" s="17"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
     </row>
-    <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="8" t="s">
+    <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:35" ht="192.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="16" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:35" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>